<commit_message>
study1 user 1 completed, study 1 user 2 started now with screen recordings
</commit_message>
<xml_diff>
--- a/Study1_User1/User1_recognition results.xlsx
+++ b/Study1_User1/User1_recognition results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="4060" windowWidth="10000" windowHeight="7980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10480" windowHeight="10860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="39">
   <si>
     <t>gesture:</t>
   </si>
@@ -129,13 +129,25 @@
   </si>
   <si>
     <t>ox</t>
+  </si>
+  <si>
+    <t>xr</t>
+  </si>
+  <si>
+    <t>xxrx</t>
+  </si>
+  <si>
+    <t>xro</t>
+  </si>
+  <si>
+    <t>xxx?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,8 +161,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +194,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -185,16 +209,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AJ34"/>
+  <dimension ref="A3:AJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="AD3" s="3" t="s">
         <v>33</v>
@@ -575,7 +602,7 @@
         <v>25</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="AH3" s="3" t="s">
         <v>33</v>
@@ -584,7 +611,7 @@
         <v>20</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
@@ -678,16 +705,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -699,37 +726,64 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P5" t="s">
         <v>15</v>
       </c>
       <c r="R5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W5" t="s">
         <v>16</v>
       </c>
       <c r="X5" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
@@ -737,57 +791,84 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6" t="s">
         <v>31</v>
       </c>
-      <c r="S6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V6" t="s">
-        <v>16</v>
-      </c>
-      <c r="W6" t="s">
-        <v>13</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="AE6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -796,16 +877,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
         <v>15</v>
@@ -814,19 +895,19 @@
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P7" t="s">
         <v>16</v>
@@ -835,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="S7" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -848,6 +929,33 @@
       </c>
       <c r="X7" t="s">
         <v>15</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
@@ -855,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -864,48 +972,75 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N8" t="s">
         <v>16</v>
       </c>
       <c r="O8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R8" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="S8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="T8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="V8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
       </c>
       <c r="X8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -914,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -926,45 +1061,72 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" t="s">
-        <v>15</v>
-      </c>
       <c r="O9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R9" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="S9" t="s">
         <v>15</v>
       </c>
       <c r="T9" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="V9" t="s">
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -973,40 +1135,40 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
         <v>15</v>
       </c>
       <c r="P10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R10" t="s">
         <v>15</v>
@@ -1018,13 +1180,40 @@
         <v>15</v>
       </c>
       <c r="V10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="X10" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
@@ -1032,58 +1221,85 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI11" t="s">
         <v>23</v>
       </c>
-      <c r="J11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" t="s">
-        <v>16</v>
-      </c>
-      <c r="R11" t="s">
-        <v>16</v>
-      </c>
-      <c r="S11" t="s">
-        <v>15</v>
-      </c>
-      <c r="T11" t="s">
-        <v>13</v>
-      </c>
-      <c r="V11" t="s">
-        <v>16</v>
-      </c>
-      <c r="W11" t="s">
-        <v>13</v>
-      </c>
-      <c r="X11" t="s">
-        <v>13</v>
+      <c r="AJ11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
@@ -1091,57 +1307,89 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="P12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" t="s">
+        <v>16</v>
+      </c>
+      <c r="X12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12" t="s">
-        <v>16</v>
-      </c>
-      <c r="P12" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" t="s">
-        <v>14</v>
-      </c>
-      <c r="S12" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" t="s">
-        <v>13</v>
-      </c>
-      <c r="V12" t="s">
-        <v>16</v>
-      </c>
-      <c r="W12" t="s">
-        <v>15</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="AD12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="X13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1210,7 +1458,7 @@
         <v>20</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="AD14" s="3" t="s">
         <v>33</v>
@@ -1219,7 +1467,7 @@
         <v>25</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="AH14" s="3" t="s">
         <v>33</v>
@@ -1228,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="AJ14" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
@@ -1321,257 +1569,465 @@
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" t="s">
-        <v>15</v>
-      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" t="s">
-        <v>15</v>
-      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" t="s">
-        <v>15</v>
-      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L20" t="s">
-        <v>15</v>
-      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" t="s">
-        <v>15</v>
-      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" t="s">
-        <v>15</v>
-      </c>
-      <c r="L22" t="s">
-        <v>15</v>
-      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" t="s">
-        <v>15</v>
-      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -1803,6 +2259,33 @@
       <c r="X27" t="s">
         <v>15</v>
       </c>
+      <c r="Z27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -1862,6 +2345,33 @@
       <c r="X28" t="s">
         <v>15</v>
       </c>
+      <c r="Z28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -1921,6 +2431,33 @@
       <c r="X29" t="s">
         <v>15</v>
       </c>
+      <c r="Z29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -1980,6 +2517,33 @@
       <c r="X30" t="s">
         <v>15</v>
       </c>
+      <c r="Z30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -2039,6 +2603,33 @@
       <c r="X31" t="s">
         <v>15</v>
       </c>
+      <c r="Z31" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -2098,8 +2689,35 @@
       <c r="X32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Z32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -2157,8 +2775,35 @@
       <c r="X33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Z33" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -2215,6 +2860,481 @@
       </c>
       <c r="X34" t="s">
         <v>21</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" t="s">
+        <v>16</v>
+      </c>
+      <c r="P38" t="s">
+        <v>15</v>
+      </c>
+      <c r="R38" t="s">
+        <v>13</v>
+      </c>
+      <c r="S38" t="s">
+        <v>16</v>
+      </c>
+      <c r="T38" t="s">
+        <v>13</v>
+      </c>
+      <c r="V38" t="s">
+        <v>16</v>
+      </c>
+      <c r="W38" t="s">
+        <v>16</v>
+      </c>
+      <c r="X38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" t="s">
+        <v>28</v>
+      </c>
+      <c r="N39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O39" t="s">
+        <v>16</v>
+      </c>
+      <c r="P39" t="s">
+        <v>15</v>
+      </c>
+      <c r="R39" t="s">
+        <v>31</v>
+      </c>
+      <c r="S39" t="s">
+        <v>16</v>
+      </c>
+      <c r="T39" t="s">
+        <v>15</v>
+      </c>
+      <c r="V39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W39" t="s">
+        <v>13</v>
+      </c>
+      <c r="X39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" t="s">
+        <v>15</v>
+      </c>
+      <c r="O40" t="s">
+        <v>16</v>
+      </c>
+      <c r="P40" t="s">
+        <v>16</v>
+      </c>
+      <c r="R40" t="s">
+        <v>15</v>
+      </c>
+      <c r="S40" t="s">
+        <v>15</v>
+      </c>
+      <c r="T40" t="s">
+        <v>15</v>
+      </c>
+      <c r="V40" t="s">
+        <v>15</v>
+      </c>
+      <c r="W40" t="s">
+        <v>15</v>
+      </c>
+      <c r="X40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" t="s">
+        <v>17</v>
+      </c>
+      <c r="N41" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" t="s">
+        <v>16</v>
+      </c>
+      <c r="P41" t="s">
+        <v>16</v>
+      </c>
+      <c r="R41" t="s">
+        <v>31</v>
+      </c>
+      <c r="S41" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41" t="s">
+        <v>16</v>
+      </c>
+      <c r="V41" t="s">
+        <v>13</v>
+      </c>
+      <c r="W41" t="s">
+        <v>15</v>
+      </c>
+      <c r="X41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K42" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" t="s">
+        <v>15</v>
+      </c>
+      <c r="N42" t="s">
+        <v>15</v>
+      </c>
+      <c r="O42" t="s">
+        <v>15</v>
+      </c>
+      <c r="P42" t="s">
+        <v>15</v>
+      </c>
+      <c r="R42" t="s">
+        <v>31</v>
+      </c>
+      <c r="S42" t="s">
+        <v>15</v>
+      </c>
+      <c r="T42" t="s">
+        <v>15</v>
+      </c>
+      <c r="V42" t="s">
+        <v>15</v>
+      </c>
+      <c r="W42" t="s">
+        <v>15</v>
+      </c>
+      <c r="X42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" t="s">
+        <v>26</v>
+      </c>
+      <c r="O43" t="s">
+        <v>15</v>
+      </c>
+      <c r="P43" t="s">
+        <v>16</v>
+      </c>
+      <c r="R43" t="s">
+        <v>15</v>
+      </c>
+      <c r="S43" t="s">
+        <v>15</v>
+      </c>
+      <c r="T43" t="s">
+        <v>15</v>
+      </c>
+      <c r="V43" t="s">
+        <v>15</v>
+      </c>
+      <c r="W43" t="s">
+        <v>13</v>
+      </c>
+      <c r="X43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" t="s">
+        <v>23</v>
+      </c>
+      <c r="J44" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" t="s">
+        <v>26</v>
+      </c>
+      <c r="O44" t="s">
+        <v>16</v>
+      </c>
+      <c r="P44" t="s">
+        <v>16</v>
+      </c>
+      <c r="R44" t="s">
+        <v>16</v>
+      </c>
+      <c r="S44" t="s">
+        <v>15</v>
+      </c>
+      <c r="T44" t="s">
+        <v>13</v>
+      </c>
+      <c r="V44" t="s">
+        <v>16</v>
+      </c>
+      <c r="W44" t="s">
+        <v>13</v>
+      </c>
+      <c r="X44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" t="s">
+        <v>17</v>
+      </c>
+      <c r="L45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45" t="s">
+        <v>15</v>
+      </c>
+      <c r="O45" t="s">
+        <v>16</v>
+      </c>
+      <c r="P45" t="s">
+        <v>16</v>
+      </c>
+      <c r="R45" t="s">
+        <v>14</v>
+      </c>
+      <c r="S45" t="s">
+        <v>16</v>
+      </c>
+      <c r="T45" t="s">
+        <v>13</v>
+      </c>
+      <c r="V45" t="s">
+        <v>16</v>
+      </c>
+      <c r="W45" t="s">
+        <v>15</v>
+      </c>
+      <c r="X45" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>